<commit_message>
Validate Supervisor Ticket List Page
</commit_message>
<xml_diff>
--- a/Excels/test.xlsx
+++ b/Excels/test.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a2388006/git/CS_PORTAL/Excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2394650\IdeaProjects\cs-portal-automation_selenium\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FEDAD4-006A-8B42-A245-B41C3AFD12E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{1FFDF3F0-6759-694F-9CB5-F32127F0BD7D}"/>
+    <workbookView xWindow="3900" yWindow="2265" windowWidth="28035" windowHeight="17445" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="TicketId" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -44,16 +44,22 @@
     <t>UserType</t>
   </si>
   <si>
-    <t>FE</t>
-  </si>
-  <si>
-    <t>Secure@2021</t>
+    <t>June@123$</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>ticketid</t>
+  </si>
+  <si>
+    <t>080720000457</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -92,9 +98,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -409,16 +416,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365E7A5F-3E6A-E248-889F-23B3A6B34B5F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,21 +436,50 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2388006</v>
+        <v>2390495</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{35F0E809-829E-5B45-8441-194CB68A33B9}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>